<commit_message>
Update browser configuration to use Firefox, enhance login step descriptions, and add new UI test scenarios for invalid and valid login cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/FullScenario_Data.xlsx
+++ b/src/test/resources/testdata/FullScenario_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SherifHamdy\Documents\GitHub\eja\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SherifHamdy\Documents\GitHub\ejadaAutomationTask\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1E11CD-21CA-41D4-A234-E3190F767CCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2C2388-F2F0-4C7F-932B-B451DEB18D09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>validUsername</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>LN</t>
+  </si>
+  <si>
+    <t>expectedThanksHeader</t>
+  </si>
+  <si>
+    <t>expectedThanksBody</t>
+  </si>
+  <si>
+    <t>Thank you for your order!</t>
+  </si>
+  <si>
+    <t>Your order has been dispatched, and will arrive just as fast as the pony can get there!</t>
   </si>
 </sst>
 </file>
@@ -381,15 +393,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74893A54-C6EE-433A-B73D-05F1648861A3}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,8 +420,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -427,6 +445,12 @@
       </c>
       <c r="F2" s="3">
         <v>12345</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>